<commit_message>
Código da adição do título e do local na planilha
</commit_message>
<xml_diff>
--- a/Vagas do Dia.xlsx
+++ b/Vagas do Dia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,443 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas Sênior</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Bilingue</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Analista de Teste</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Analista Jurídico Pl II</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Analista BI</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Scrum Master</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Tech Lead - Mobile</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Agile Master</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Mobile - Flutter</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Engenheiro de Software Java Especialista</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Móbile Sênior</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Backend Sr</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Engenheiro de Software Sr (.NET Core e/ou Node.js)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Analista SOA.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UX/UI Designer Pleno</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Back End NodeJS</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Scrum Master</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Scrum Master</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET/Oracle</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Tech Lead</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>QA com conhecimento em Jest</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Desenvolvedor RPA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FontEnd React</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Back End Java</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Analista de Processos RPA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Analista de NOC Jr III</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Dev Peoplesoft - ERP</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Estágio Logistica</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Estágio em TI</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Especialista em QA</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Lider Técnico</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Analista Service Desk Jr I</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Desenvolvedor BackEnd Java - Springboot</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morumbi - SP </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
coleta do local das vagas
</commit_message>
<xml_diff>
--- a/Vagas do Dia.xlsx
+++ b/Vagas do Dia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,114 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adcionado a coleta da descrição das vagas
</commit_message>
<xml_diff>
--- a/Vagas do Dia.xlsx
+++ b/Vagas do Dia.xlsx
@@ -440,111 +440,296 @@
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Morumbi - SP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Alphaville - SP</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Alphaville - SP</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Home office</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>home office</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Home office</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>São Judas - SP</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>São Judas - SP</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Home Office</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Inserindo a descrição na planilha
</commit_message>
<xml_diff>
--- a/Vagas do Dia.xlsx
+++ b/Vagas do Dia.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="2022-01-19" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2022-01-20" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -439,7 +439,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Analista de Sistemas Sênior</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Morumbi - SP</t>
@@ -447,287 +451,602 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Teste</t>
+          <t>• Conhecimento avançado em UML; • Experiência linguagem Java; • Experiência com frameworks Java como Spring, Springboot, Hibernate, Junit, Angular; • Experiência com Servidores de aplicação Jboss, Tomcat, Jetty; • Experiência com Oracle; • Experiência com Integração Continua e Entrega Continua; • Experiência com ferramenta Git; • Experiência com monolíticos e microsserviços;</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Analista de Infraestrutura Bilingue</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Alphaville - SP</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Experiência com Linux - avançado; Inglês- avançado para conversação;</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Analista de Teste</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Requisitos: Avaliação de requisitos de testes. Definição de estratégia de testes. Planejamento de testes. Execução de testes funcional. Monitoramento e reporte de testes. Verificações em especificações de requisitos de sistemas / software.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Analista Jurídico Pl II</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Alphaville - SP</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Responsabilidades: Triagem das notificações emitidas por órgãos e direcionamento às áreas de atuação. Follow up com áreas de atuação para encerramento das obrigações no sistema com base em evidências. Suporte nas demandar administrativas como elaboração de relatórios. Atas e apresentações. Dar suporte às lojas para acessar o sistema Archer e outros. Formação: Formado ou cursando Direito</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Analista BI</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Skills da vaga: - QlikView; - QlikSense; - Tableau; - Power BI; - Looker; - Superset; - Kibana. Analista de Dados/BI Skills da vaga: - Banco de Dados (DML/DDL) - SQL Server - Modelagem de Dados Relacional e Multidimensional. - ETL e automação (Integration Services) - BI (Cubos OLAP) - Git - Queries SQL, bancos relacionais e conhecimento de ecossistema Hadoop.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Scrum Master</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Scrum Master   Descrição das atividades   O que você precisa ter: Conhecimento em Scrum, cerimônias: planning, refinamento, retro, review, conhecimento em Jira e Confluence. Obrigatório:Experiência como Scrum Master Domínio sobre o Framework Scrum (Papeis, Artefatos, Cerimônias, etc) Experiência em projetos de tecnologia Visão crítica e analítica Desejável: Conhecimento em Kanban Experiência na análise e geração de métricas/indicadores; Diferencial: Certificações Ágeis   Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Tech Lead - Mobile</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Home office</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tech Lead, com experiencia com Mobile Nativo + Android + Ios</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Agile Master</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Agile Master   Descrição das atividades   O que você precisa ter: Vivencia em liderança de times com práticas Scrum e Kanban, facilitando dinâmicas e fluxo de trabalho da equipe, focando em entregas com excelência.   Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Mobile - Flutter</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>home office</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Possuir conhecimentos com Desenvolvimento Flutter e GIT</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Engenheiro de Software Java Especialista</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Engenheiro de Software Java Especialista.   Descrição das atividades   Skill Técnico solicitado: Conhecimentos sólidos de Java 8 e 11 Experiência com o Spring Framework (Boot, Data, Cloud, Cloud Streams) Experiência com PostgreSQL Experiência com banco NoSQL (MongoDB, ElasticSearch) Experiência com Redis Experiência com arquitetura de microsserviços Experiência com clean architecture ou hexagonal Experiência com message broker (Kafka ou RabbitMQ) Domínio de design patterns Conhecimento sólido de processos de CI/CD Experiência com escrita de testes unitário e integrado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Móbile Sênior</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Desenvolvedor Móbile Sênior.   Descrição das atividades   Skill Técnico solicitado: 3+ anos de experiência profissional em desenvolvimento de software - Experiência na criação de soluções móveis React Native ou Flutter para Android e iOS - Domínio firme da linguagem JavaScript e suas nuances, incluindo sintaxe ES6 + - Capacidade de escrever código Javascript limpo e bem documentado - Familiaridade com ferramentas de compilação nativas, como XCode, Gradle - Compreensão de APIs REST e armazenamento offline - Experiência com suítes de testes automatizados - Administração e implantação das lojas Play Store e App Store; - (CI / CD) para React Native ou Flutter. Diferenciais Experiência com aplicações de larga escala; Experiência em arquitetura de software ou liderança de equipe.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Backend Sr</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Desenvolvedor Backend Sr.   Descrição das atividades   Skill Técnico solicitado: Sólidos conhecimentos nas linguagens de Javascript e Java; ●Sólidos conhecimentos em algoritmos e estrutura de dados; ●Experiência em automação e orquestração de contêineres, utilizando tecnologias como Docker e Kubernetes; ●Bons conhecimentos em Git; ●Bons conhecimentos em Linux e Bash Script; ●Boa comunicação e facilidade de lidar com o trabalho em equipes remotas. ●Bons conhecimentos em bancos relacionais e não relacionais como MySQL e MongoDB. Diferenciais Não que seja imprescindível, mas você pode se destacar bastante se tiver: ●Experiência em Spark, Scala, PHP e/ou Python; ●Experiência de atuação em produtos/sistemas de internet críticos e escaláveis; ●Experiência em projetar e desenvolver APIs REST, utilizando Node.js; ●Experiência com ferramentas de automação de infraestrutura (Ansible/Terraform); ●Experiência com estratégias de caching, utilizando Redis Cache; ●Capacidade de avaliar, discutir, definir e propor melhorias para a arquitetura de nossos sistemas; ●Conhecimentos em SOLID; ●Conhecimentos em CI/CD; ●Conhecimentos em Azure Cloud e/ou AWS Cloud.   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Engenheiro de Software Sr (.NET Core e/ou Node.js)</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Engenheiro de Software Sr (.NET Core e/ou Node.js).   Descrição das atividades   Skill Técnico solicitado: Ser proativo e ter boa comunicação com o time; -Fluência nas linguagens de programação .NET Core e/ou Node.js; -Experiência em times ágeis (SCRUM ou Kanban); -Experiência com Design Patterns; -Experiência em desenvolvimento de APIs; -Experiência com Unit Test para .NET e/ou Node.js; -Experiência com desenvolvimento de aplicações conteinerizadas de alta disponibilidade (ECS ou Kubernetes); -Experiência com armazenamento de dados NoSQL (DynamoDB ou outro) -Experiência com Cloud AWS; -Experiência em desenvolvimento e uso de serverless (AWS Lambdas) -Conhecimentos em tecnologias como S3, ELB, Api Gateway; -Conhecimento de CI e CD; -Capacidade de análise de monitorias usando CloudWatch/Grafana. Você fica em evidência com: -Experiência com Streaming ou mensageria (SQS ou outro) ou -Experiência com ElasticSearch ou outro sistema de analytics/searches ou -Experiência com Redis e/ou outro sistema de cache ou -Experiência com linguagem de programação Typescript ou -Experiência com arquitetura de software visando estabilidade, performance e escalabilidade ou -Conhecimentos de DevOps.</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Analista SOA.</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Analista SOA.   Descrição das atividades   Skill Técnico solicitado: Linguagem orientada a Objetos (Java/.NET); PHP; JavaScript; BIG MACHINE LANGUAGE (BML) para Oracle CPQ Cloud; Integrações envolvendo SOAP/REST; Linux (Intermediário) de acesso a arquivos, logs e monitoramento; SOA/Oracle e integrações envolvendo WebLogic (OSB/ESS); Oracle Service Cloud (OSvC/Right Now). Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UX/UI Designer Pleno</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Designer Pleno   Descrição das atividades   O que você precisa ter: Requisitos e qualificações - Experiência em design de interfaces / interação; - Habilidades em UI e UX demonstradas em portfólio; - Experiência em ferramentas para execução de entregas (Adobe, Figma, etc.); - Habilidade para defender ideias e propostas de solução; - Experiência em wireframes, layouts e documentação de UX; - Excelente comunicação para interlocução com stakeholders Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Back End NodeJS</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>Home office</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Desenvolvedor Back End NodeJs   Descrição das atividades   O que você precisa ter: Conhecimento em Node JS   Skill Técnico solicitado: Vivência com atuação em squad mutidisciplinar, atuando com Scrum e Kanban Java e Cloud Functions (desejável) Home Office, Por tempo indeterminado.   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Scrum Master</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Scrum Master   Descrição das atividades   O que você precisa ter: Conhecimento em Scrum, cerimônias: planning, refinamento, retro, review, conhecimento em Jira e Confluence. Obrigatório:Experiência como Scrum Master Domínio sobre o Framework Scrum (Papeis, Artefatos, Cerimônias, etc) Experiência em projetos de tecnologia Visão crítica e analítica Desejável: Conhecimento em Kanban Experiência na análise e geração de métricas/indicadores; Diferencial: Certificações Ágeis   Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Scrum Master</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Scrum Master   Descrição das atividades   O que você precisa ter: Conhecimento em Scrum, cerimônias: planning, refinamento, retro, review, conhecimento em Jira e Confluence. Obrigatório:Experiência como Scrum Master Domínio sobre o Framework Scrum (Papeis, Artefatos, Cerimônias, etc) Experiência em projetos de tecnologia Visão crítica e analítica Desejável: Conhecimento em Kanban Experiência na análise e geração de métricas/indicadores; Diferencial: Certificações Ágeis   Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Desenvolvedor .NET   Descrição das atividades   O que você precisa ter: Necessário: - Experiência de no mínimo 2 anos atuando com .NET Core Conhecimentos: .NET Core, .Net Framework 4.5 Banco de dados Oracle, e SQL Server   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Desenvolvedor .NET/Oracle</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Analista Desenvolvedor .NET/Oracle Pleno   Descrição das atividades   O que você precisa ter: Linguagens de programação: - Sólidos conhecimentos em SQL (oracle) para fazer buscas e manipulações de tabelas - Conhecimentos em C# para analisar regras de negócio Estruturas de código: - Conhecimentos em aplicações ASP .Net MVC para análise de regras de negócio - Conhecimentos em Webforms para análise de regras de negócio - Conhecimentos em Stored Procedures e Functions utilizando a sintaxe do Oracle   Skill Técnico solicitado: Outros: - Experiência em depuração de código Oracle utilizando PL/SQL (ou equivalente) Diferenciais: - Experiência anterior atuando como desenvolvedor .Net Home Office, Por tempo indeterminado.   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Tech Lead</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Tech Lead, com experiencia com Mobile Nativo + Android + Ios</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>QA com conhecimento em Jest</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para QA com conhecimento em Jest   Descrição das atividades   O que você precisa ter: - Experiência de testes automatizados - JEST ; - Experiência com ferramentas de versionamento de código (GIT,...); - Conhecimento em metodologias ágeis (Scrum/Kanban);   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Desenvolvedor RPA</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Desenvedor RPA   Descrição das atividades   O que você terá que fazer: Mapear processos para automação juntamente com a área de negócio; Desenvolver automações RPA usando Power Automate; Dar sustentação e/ou aprimorar automações já existentes; Desenvolver rotinas de manipulação de dados vindos de planilhas, pdf, txt e etc; Homologação de tarefas automatizadas junto aos usuários; Obrigatório: Experiência com Power Automate; Conhecimentos sobre RPA; Desejável: Experiência com Python; Conhecimento em desenho de processos de automação e especificações técnicas; Diferencial: Certificação Power Automate (PL-900) ou conhecimento comprovado Experiência com outras ferramentas de automação (UiPath, Automation Edge, Etc); Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Full Stack</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Desenvolvedor Full Stack Pleno Sênior   Descrição das atividades   O que você precisa ter: Experiência com .Net e Angular   Skill Técnico solicitado: Desejavel: Python, Xamarim, MongoDB, Postgre e Oracle   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FontEnd React</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Desenvolvedor FrontEnd React   Descrição das atividades   O que você precisa ter: - Sólidos conhecimentos técnicos em React - Sólidos conhecimentos técnicos em NextJS - Sólidos conhecimentos técnicos em Node - Experiência atuando com React em projetos grandes - Conhecimentos em GraphQL - Conhecimentos sobre arquitetura e boas práticas de desenvolvimento web - Noções sobre ambientes AWS   Skill Técnico solicitado: - Atuação em projetos de E-Commerce - Conhecimentos em React Native - Conhecimentos em Java (spring e springboot) - Conhecimentos em Kubernetes - Conhecimentos em PostgreSQL - Conhecimentos em Apache Cassandra - Conhecimentos/especializações em UI/UX   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Desenvolvedor Back End Java</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Desenvolvedor Back End Java   Descrição das atividades   O que você precisa ter: Necessário: - Sólidos conhecimentos técnicos em Java 11 ao 14 - Sólidos conhecimentos técnicos em Spring, Springboot e microserviços - Experiência atuando com springboot e kubernetes em projetos grandes - Conhecimentos em Kubernetese Postgres - Conhecimentos sobre arquitetura e boas práticas de desenvolvimento backend - Noções sobre ambientes AWS   Skill Técnico solicitado: Interessante: - Atuação em projetos de E-Commerce - Certificações de Java - Conhecimentos em Apache Cassandra, React, React Native, Node, GraphQL Home Office – Tempo indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Analista de Processos RPA</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Analista de Processos RPA   Descrição das atividades   O que você precisa ter: Mapear processos para automação juntamente com as áreas de negócio (AS-IS x TO-BE); Redigir documentação técnica de processos (PDD); Apoiar no pré venda de soluções RPA (reunião com clientes, elaboração de propostas, etc). Obrigatório: Experiência em mapeamento e modelagem de processos; Criação e manipulação de apresentações PowerPoint (.pptx) de qualidade visual; Conhecimentos em ferramentas de mapeamento de processos (ex: Bizagi, Visio, etc); Domínio da língua portuguesa e excelente comunicação oral e escrita. Desejável: Conhecimento em automação de processos RPA. Diferencial: Conhecimento em ferramentas de automação RPA (AutomationEdge, UiPath, etc Home Office – Tempo Indeterminado   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Analista de NOC Jr III</t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Analista de NOC Jr III   Descrição das atividades   Skill Técnico solicitado: Ao mínimo 2 anos de experiência atuando no noc; Conhecimentos em Zabbix, Jira, Grafana e Solarwinds; Vivência em servidores Windows; Inglês Nível Intermediário. Diferencial: Conhecimentos em servidores Linux.   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Dev Peoplesoft - ERP</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Dev Peoplesoft - ERP   Descrição das atividades   Skill Técnico solicitado: Application Designer, PeopleCode, Application Engine, Application Messaging, Component Interface, XML Publisher, SQR, Query, WorkFlow AWE, Component Interface, Application Package, Data Mover, File Layout, Programação PL/SQL. Conhecimento funcional desejável nos módulos do ERP Peoplesoft: o BI, AR, PO, AP, GL, TR, AM.   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Estágio Logistica</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>São Judas - SP</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Estágio Logistica   Descrição das atividades   O que você terá que fazer: Controle de ativos que entram e saem do estoque.   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Estágio em TI</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>São Judas - SP</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Estágio TI   Descrição das atividades   O que você terá que fazer: "Profissional irá atuar na área de Suporte Técnico à Usuário N2, manutenção preventiva e corretiva de notebooks e periféricos. Realizará a instalação e configuração de aplicativo, verificação hardware e instalação de sistema operacional. Análises de equipamentos de troca ou desligamento, substituição de processadores, fontes, hd, memórias. Controle de ativos que entram e saem do estoque. • Área e especialização profissional: Informática, TI, Telecomunicações - TI, Logistica, Administração • Nível hierárquico: Estagiário • Local de trabalho: São Judas - SP   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida).</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Especialista em QA</t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Especialista em QA   Descrição das atividades   O que você precisa ter: 5 anos + Experiencia em Desenvolvimento. Acompanhamento e realização de testes nas aplicações/softwares e aplicativos garantindo as qualidade e funcionalidades desenvolvidas com reportes das evoluções   O que você terá que fazer: . Realização dos testes progressivos e regressivos das versões dos aplicativos, backend e demais ferramentas de suporte. Especificação e automatização dos testes. Geração, integração e entrega das versões. Atuar na interface entre o cliente e a empresa na definição das metodologias e execução de testes. Definição e implementação de critérios de aceite e qualidade de software. Definição e implementação de métricas para medição dos processos de testes. Estudo de causa raiz, mapeamento dos incidentes problemas e endereçamento das correções. Execução e controle de Testes, validação das soluções e controle de versões   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Lider Técnico</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Lider Técnico   Descrição das atividades   O que você terá que fazer: Interagir constantemente com os usuários de forma a garantir melhor compreensão; Desenvolver, testar e homologar solução definida; Identificar possíveis erros e demonstrar proatividade para resolvê-los da solução; Garantir em conjunto com a equipe o alcance das entregas definidas para a equipe; Liderar a equipe técnicamente, mostrando o caminho e resolvendo problemas; Requerimentos: Experiência com desenvolvimento de sistemas (Backend e Frontend) Experiência em .Net Core, Angular; Experiência com SQL Server; Vivência em times com desenvolvimento de metodologia Ágil e conhecimento contábil serão considerados diferenciais; Ter atuado como referente técnico ou líder de equipe técnica;   • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Analista Service Desk Jr I</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Analista Service Desk Jr I   Descrição das atividades   O que você terá que fazer: Receber os chamados de suporte abertos pelos usuários dos clientes cadastrados no sistema de gerenciamento ou encaminhados pelos Analistas de Service Desk; Realizar avaliação preliminar dos incidentes gerados, contatar o usuário para identificar a solução; Executar os processos para avaliação e identificação de problemas nos equipamentos dos usuários garantindo a sua satisfação;   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Desenvolvedor BackEnd Java - Springboot</t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>Home Office</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   Atualmente estamos com oportunidade para Desenvolvedor Back End Java – Springboot   Descrição das atividades   O que você terá que fazer: Atuar com a sustentação de APIs em Java 11 utilizando Springboot que estão publicadas na AWS como lambdas. - Desenvolver novas APIs em Java com springboot e publicá-las na AWS como lambdas.   Skill Técnico solicitado Necessário: - Experiência construindo e mantendo aplicações criadas em Java 8+ com Springboot. - Experiência utilizando o console da AWS. - Conhecimentos em OpenApi. - Conhecimentos em Lambdas (AWS). - Conhecimentos em API Gateway (AWS). Interessante: - Experiência com configuração de recursos da AWS. - Experiência criando ou mantendo aplicações Java com OpenApi. - Experiência com JSF. - Conhecimentos em Angular 6+. - Conhecimentos em testes unitários. Experiência: - Mínimo de 3 anos atuando na área de desenvolvimento. - Mínimo de 2 anos atuando com Springboot.   Dê um play em sua carreira! #VemSerCadmus.</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Desenvolvedor FullStack</t>
+        </is>
+      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Somos uma das melhores empresas para trabalhar pelo GPTW, por isso, buscamos os melhores talentos porque acreditamos que só com pessoas incríveis entregamos resultados incríveis.   E aí, topa transformar ideias em potência com propósito de impactar a sociedade com a gente? Então faça parte de uma empresa que tem seus processos guiados por seus valores, valoriza seus colaboradores, sempre pensando no desenvolvimento profissional de cada um. E disponibiliza ambientes descontraídos, para que todos se sintam respeitados, acolhidos e acima de tudo: felizes.   Atualmente estamos com oportunidade para Desenvolvedor FullStack   Nossos Diferencias: • Acompanhamento e desenvolvimento de carreira • Programa de pontos onde você escolhe seus benefícios (Plano de saúde, odontológico, vale alimentação, vale refeição, seguro de vida). • Treinamento e capacitação • Portal de conhecimentos e práticas • COP (Comunidade de Prática) • Clube de vantagens Lincard (Em casos de PJ ) • E muito mais….   Dê um play em sua carreira! #VemSerCadmus.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajuste das dimensões das colunas da planilha
</commit_message>
<xml_diff>
--- a/Vagas do Dia.xlsx
+++ b/Vagas do Dia.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,19 +424,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="70" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Local</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Descrição</t>
         </is>

</xml_diff>